<commit_message>
Modificaciones Pertinentes a la última Semana. Se agrega el documento integrador. Se acabó, jóvenes :D
</commit_message>
<xml_diff>
--- a/Docs/Línea de Tiempo.xlsx
+++ b/Docs/Línea de Tiempo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaiduck\Downloads\Dropbox\Escuela\Informática\Administración de Proyectos\Proyecto Despacho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaiduck\Downloads\GitHub\Administración\AdminProyectos\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -393,6 +393,53 @@
 </comments>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>1.- Lista de Acontecimientos</t>
+  </si>
+  <si>
+    <t>2.- Diagrama de Flujo</t>
+  </si>
+  <si>
+    <t>3.- Diagrama E-R</t>
+  </si>
+  <si>
+    <t>4. Modelo de Base de Datos</t>
+  </si>
+  <si>
+    <t>5.-Primera Forma Normal</t>
+  </si>
+  <si>
+    <t>6.- Segunda Forma Normal</t>
+  </si>
+  <si>
+    <t>7.- Tercera Forma Normal</t>
+  </si>
+  <si>
+    <t>8.- Esquema de Base de Datos</t>
+  </si>
+  <si>
+    <t>9.- Creación de Base de Datos</t>
+  </si>
+  <si>
+    <t>10.- Diccionario de Base de Datos</t>
+  </si>
+  <si>
+    <t>11.- Puntos de Función</t>
+  </si>
+  <si>
+    <t>12.- Modelo de Tareas</t>
+  </si>
+  <si>
+    <t>13.- Prototipo de Ventanas</t>
+  </si>
+  <si>
+    <t>14.- Codificación de Ventanas</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
@@ -425,7 +472,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -442,11 +489,56 @@
         <color auto="1"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,6 +547,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,16 +1330,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>310243</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>10885</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>311605</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>20410</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1247,9 +1347,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8235043" y="201385"/>
-          <a:ext cx="1362" cy="200025"/>
+        <a:xfrm flipH="1">
+          <a:off x="6477000" y="201385"/>
+          <a:ext cx="1758043" cy="1817915"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1274,16 +1374,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>315685</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>317047</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1291,9 +1391,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8850085" y="190500"/>
-          <a:ext cx="1362" cy="200025"/>
+        <a:xfrm flipH="1">
+          <a:off x="6715125" y="190500"/>
+          <a:ext cx="2134960" cy="1895475"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1318,16 +1418,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>310242</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>311604</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1335,53 +1435,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10673442" y="190499"/>
-          <a:ext cx="1362" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>306161</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="98" name="Straight Connector 97"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11277599" y="190499"/>
-          <a:ext cx="1362" cy="200025"/>
+        <a:xfrm flipH="1">
+          <a:off x="7305676" y="238125"/>
+          <a:ext cx="2152649" cy="2057400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2009,6 +2065,168 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5991225" y="1792061"/>
+          <a:ext cx="168729" cy="141514"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>39460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>464004</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Oval 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6391275" y="1944460"/>
+          <a:ext cx="168729" cy="141514"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>121104</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>65314</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Oval 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6657975" y="2019300"/>
+          <a:ext cx="168729" cy="141514"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>121104</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>55788</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Oval 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7267575" y="2200274"/>
           <a:ext cx="168729" cy="141514"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2308,72 +2526,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U21"/>
+  <dimension ref="B1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C1" s="1">
+      <c r="C1" s="7">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="7">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="7">
         <v>3</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="7">
         <v>4</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="7">
         <v>5</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="7">
         <v>6</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1" s="7">
         <v>7</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="7">
         <v>8</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1" s="7">
         <v>9</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="7">
         <v>10</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M1" s="7">
         <v>11</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N1" s="7">
         <v>12</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1" s="7">
         <v>13</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="7">
         <v>14</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1" s="7">
         <v>15</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R1" s="7">
         <v>16</v>
       </c>
-      <c r="S1" s="1">
-        <v>17</v>
-      </c>
+      <c r="S1" s="1"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
@@ -2395,7 +2627,7 @@
       <c r="S3" s="1"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
@@ -2417,7 +2649,7 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
       <c r="C5" s="1"/>
@@ -2439,7 +2671,7 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
+      <c r="B6" s="7">
         <v>4</v>
       </c>
       <c r="C6" s="1"/>
@@ -2461,7 +2693,7 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
@@ -2483,7 +2715,7 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+      <c r="B8" s="7">
         <v>6</v>
       </c>
       <c r="C8" s="1"/>
@@ -2505,7 +2737,7 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
+      <c r="B9" s="7">
         <v>7</v>
       </c>
       <c r="C9" s="1"/>
@@ -2527,7 +2759,7 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
+      <c r="B10" s="7">
         <v>8</v>
       </c>
       <c r="C10" s="1"/>
@@ -2549,7 +2781,7 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
+      <c r="B11" s="7">
         <v>9</v>
       </c>
       <c r="C11" s="1"/>
@@ -2571,7 +2803,7 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
+      <c r="B12" s="7">
         <v>10</v>
       </c>
       <c r="C12" s="1"/>
@@ -2593,7 +2825,7 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
+      <c r="B13" s="7">
         <v>11</v>
       </c>
       <c r="C13" s="1"/>
@@ -2615,7 +2847,7 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
+      <c r="B14" s="7">
         <v>12</v>
       </c>
       <c r="C14" s="1"/>
@@ -2637,7 +2869,7 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
+      <c r="B15" s="7">
         <v>13</v>
       </c>
       <c r="C15" s="1"/>
@@ -2659,7 +2891,7 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
+      <c r="B16" s="7">
         <v>14</v>
       </c>
       <c r="C16" s="1"/>
@@ -2678,7 +2910,7 @@
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+      <c r="B17" s="7">
         <v>15</v>
       </c>
       <c r="C17" s="1"/>
@@ -2697,7 +2929,7 @@
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
+      <c r="B18" s="7">
         <v>16</v>
       </c>
       <c r="C18" s="1"/>
@@ -2719,7 +2951,7 @@
       <c r="U18" s="1"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
+      <c r="B19" s="7">
         <v>17</v>
       </c>
       <c r="C19" s="1"/>
@@ -2741,16 +2973,62 @@
       <c r="U19" s="1"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>